<commit_message>
Cleaned up exception handling to more consistenly leverage ApodeixiError's functional tracing. Supported comments in parenthenis in entity names
</commit_message>
<xml_diff>
--- a/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
+++ b/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DC0E21-6C79-4FFC-B3F9-DC3FAA0E0339}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08ECA4E-C612-4BEF-AF25-AF52E6388534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
   <si>
     <t>Big Rock</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>My Corp</t>
-  </si>
-  <si>
-    <t>Effort</t>
   </si>
 </sst>
 </file>
@@ -917,7 +914,7 @@
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -961,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="24" t="s">
@@ -2565,6 +2562,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F6243DC9F1A5042A9E247A4534B7346" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d7c915ce63f17b192f15f9b5c7111dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16245bed-a411-4918-92cd-ff4510683069" xmlns:ns3="ddeece39-a33c-49ad-a8fd-0ae9fa2c3195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="06dc0855dc4fc49148f60a39d2bf92c3" ns2:_="" ns3:_="">
     <xsd:import namespace="16245bed-a411-4918-92cd-ff4510683069"/>
@@ -2781,15 +2787,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
   <ds:schemaRefs>
@@ -2800,6 +2797,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22B48C8D-ED50-492C-9680-7011CC9B9CB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2816,12 +2821,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added ability to link manifests posted together, like effort and big rocks
</commit_message>
<xml_diff>
--- a/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
+++ b/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08ECA4E-C612-4BEF-AF25-AF52E6388534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1284DB-4B6C-406D-8D88-E11715849571}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="76">
   <si>
     <t>Big Rock</t>
   </si>
@@ -245,9 +245,6 @@
     <t>E2:F9</t>
   </si>
   <si>
-    <t>Big Rock Estimates</t>
-  </si>
-  <si>
     <t>Investment</t>
   </si>
   <si>
@@ -255,6 +252,18 @@
   </si>
   <si>
     <t>My Corp</t>
+  </si>
+  <si>
+    <t>data.kind.3</t>
+  </si>
+  <si>
+    <t>data.range.3</t>
+  </si>
+  <si>
+    <t>F2:F9</t>
+  </si>
+  <si>
+    <t>Big Rock Estimate</t>
   </si>
 </sst>
 </file>
@@ -914,7 +923,7 @@
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1102,7 +1111,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="12"/>
@@ -1131,7 +1140,7 @@
         <v>66</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13">
@@ -1148,7 +1157,7 @@
         <v>67</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1159,10 +1168,10 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="32" t="s">
         <v>72</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1173,69 +1182,81 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>19</v>
+        <v>63</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>71</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>23</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>19</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="29">
-        <v>44315</v>
+        <v>25</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="29">
+        <v>44315</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
@@ -2556,18 +2577,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2788,18 +2809,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>